<commit_message>
Add protobuf dumper support.
</commit_message>
<xml_diff>
--- a/test/input/ActorConf.xlsx
+++ b/test/input/ActorConf.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\xls2lua\test\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vyronlee/Workspace/XlsxConverter/test/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C95701C-6A1F-6240-BDE7-02CA065816A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12840"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Properties" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -125,19 +126,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -171,7 +172,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -448,16 +449,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -497,7 +498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -517,7 +518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -537,7 +538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -557,7 +558,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -577,7 +578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>

</xml_diff>